<commit_message>
Actualización del cronograma del proyecto
La modificación se realizó debido al retiro de uno de los integrantes del equipo.
</commit_message>
<xml_diff>
--- a/Desarrollo/SVCE/Documentos/SVCE-CP.xlsx
+++ b/Desarrollo/SVCE/Documentos/SVCE-CP.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="INTEGRANTES  ROLES" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name=" CRONOGRAMA" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Copia de  CRONOGRAMA" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="187">
   <si>
     <t>EQUIPO 6</t>
   </si>
@@ -286,8 +287,7 @@
     <t>Velarde Huancahuari / Programador Frontend</t>
   </si>
   <si>
-    <t xml:space="preserve">Especificar Requisito 3 -  Búsqueda de cliente para generar un reporte.
-</t>
+    <t>Especificar Requisito 3 -  Búsqueda de cliente para generar un reporte.</t>
   </si>
   <si>
     <t>Documento de Especificación de Requisitos 3</t>
@@ -449,118 +449,204 @@
     <t>Fase de programación para requisito 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Velarde Huancahuari / Programador Frontend   ---- Cristhian </t>
+  </si>
+  <si>
+    <t>Implementación de Requisito 3 - Búsqueda de cliente para generar un reporte.</t>
+  </si>
+  <si>
+    <t>Fase de programación para requisito 3</t>
+  </si>
+  <si>
+    <t>Diseño de Software 2</t>
+  </si>
+  <si>
+    <t>Documento del Diseño del Software 2</t>
+  </si>
+  <si>
+    <t>SVCE-DDS-2.DOCX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopez Salinas / Diseñador UX , Tupac Agüero / Arquitecto de Software </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>AAa</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Agreagr textlist y botón para busqueda </t>
+    </r>
+  </si>
+  <si>
+    <t>Implementación de Requisito 4 - Búsqueda y filtrado de productos.</t>
+  </si>
+  <si>
+    <t>Fase de programación para requisito 4</t>
+  </si>
+  <si>
+    <t>Implementación de Requisito 5 - Selección y compra de artículos mediante un carrito de compras.</t>
+  </si>
+  <si>
+    <t>Fase de programación para requisito 5</t>
+  </si>
+  <si>
+    <t>Implementación de Requisito 6 - Edición del listado de compras durante la compra.</t>
+  </si>
+  <si>
+    <t>Fase de programación para requisito 6</t>
+  </si>
+  <si>
+    <t>Diseño de Software 3</t>
+  </si>
+  <si>
+    <t>Documento del Diseño del Software 3</t>
+  </si>
+  <si>
+    <t>SVCE-DDS-3.DOCX</t>
+  </si>
+  <si>
+    <t>Fin: 05/06/2023</t>
+  </si>
+  <si>
+    <t>Análisis y Verificación del Hito 2</t>
+  </si>
+  <si>
+    <t>Documento de Verificación de Hito 2</t>
+  </si>
+  <si>
+    <t>SVCE-DVH-2.DOCX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liñán Paredes / Analista Junior ,  Anaya Sánchez / Analista Senior </t>
+  </si>
+  <si>
+    <t>Inicio: 06/05/2023</t>
+  </si>
+  <si>
+    <t>Implementación de Requisito 7 - Contar con diferentes medios de pago que confirmen la compra.</t>
+  </si>
+  <si>
+    <t>Fase de programación para requisito 7</t>
+  </si>
+  <si>
+    <t>HITO 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementación de Requisito 8 - Reporte de compra que permita al usuario solicitarlo. </t>
+  </si>
+  <si>
+    <t>Fase de programación para requisito 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementación de Requisito 9 -  Soporte al cliente efectivo para resolver cualquier problema. </t>
+  </si>
+  <si>
+    <t>Análisis y Verificación del Hito 3</t>
+  </si>
+  <si>
+    <t>Documento de Verificación de Hito 3</t>
+  </si>
+  <si>
+    <t>SVCE-DVH-3.DOCX</t>
+  </si>
+  <si>
+    <t>Validación del Hito 1-3</t>
+  </si>
+  <si>
+    <t>Documento de Revisión y Validación de Hitos</t>
+  </si>
+  <si>
+    <t>SVCE-DRVH.DOCX</t>
+  </si>
+  <si>
+    <t>Fin: 30/06/2023</t>
+  </si>
+  <si>
+    <t>Elaboración de Acta de Cierre de Proyecto</t>
+  </si>
+  <si>
+    <t>Acta de Cierre del Proyecto</t>
+  </si>
+  <si>
+    <t>SVCE-ACP.DOCX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 - 26 de este mes </t>
+  </si>
+  <si>
+    <t>Marco  - Cliente      / Jefferson</t>
+  </si>
+  <si>
+    <t>Itachi - Admin   / Bryan</t>
+  </si>
+  <si>
+    <t>27 - 31 de este mes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Velarde Huancahuari / Programador Frontend </t>
   </si>
   <si>
-    <t>Implementación de Requisito 3 - Búsqueda de cliente para generar un reporte.</t>
-  </si>
-  <si>
-    <t>Fase de programación para requisito 3</t>
-  </si>
-  <si>
-    <t>Diseño de Software 2</t>
-  </si>
-  <si>
-    <t>Documento del Diseño del Software 2</t>
-  </si>
-  <si>
-    <t>SVCE-DDS-2.DOCX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lopez Salinas / Diseñador UX , Tupac Agüero / Arquitecto de Software </t>
-  </si>
-  <si>
-    <t>Implementación de Requisito 4 - Búsqueda y filtrado de productos.</t>
-  </si>
-  <si>
-    <t>Fase de programación para requisito 4</t>
-  </si>
-  <si>
-    <t>Implementación de Requisito 5 - Selección y compra de artículos mediante un carrito de compras.</t>
-  </si>
-  <si>
-    <t>Fase de programación para requisito 5</t>
-  </si>
-  <si>
-    <t>Implementación de Requisito 6 - Edición del listado de compras durante la compra.</t>
-  </si>
-  <si>
-    <t>Fase de programación para requisito 6</t>
-  </si>
-  <si>
-    <t>Diseño de Software 3</t>
-  </si>
-  <si>
-    <t>Documento del Diseño del Software 3</t>
-  </si>
-  <si>
-    <t>SVCE-DDS-3.DOCX</t>
-  </si>
-  <si>
-    <t>Fin: 05/06/2023</t>
-  </si>
-  <si>
-    <t>Análisis y Verificación del Hito 2</t>
-  </si>
-  <si>
-    <t>Documento de Verificación de Hito 2</t>
-  </si>
-  <si>
-    <t>SVCE-DVH-2.DOCX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liñán Paredes / Analista Junior ,  Anaya Sánchez / Analista Senior </t>
-  </si>
-  <si>
-    <t>Inicio: 06/05/2023</t>
-  </si>
-  <si>
-    <t>Implementación de Requisito 7 - Edición del listado de compras durante la compra.</t>
-  </si>
-  <si>
-    <t>Fase de programación para requisito 7</t>
-  </si>
-  <si>
-    <t>HITO 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementación de Requisito 8 - Reporte de compra que permita al usuario solicitarlo. </t>
-  </si>
-  <si>
-    <t>Fase de programación para requisito 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementación de Requisito 9 -  Soporte al cliente efectivo para resolver cualquier problema. </t>
-  </si>
-  <si>
-    <t>Análisis y Verificación del Hito 3</t>
-  </si>
-  <si>
-    <t>Documento de Verificación de Hito 3</t>
-  </si>
-  <si>
-    <t>SVCE-DVH-3.DOCX</t>
-  </si>
-  <si>
-    <t>Validación del Hito 1-3</t>
-  </si>
-  <si>
-    <t>Documento de Revisión y Validación de Hitos</t>
-  </si>
-  <si>
-    <t>SVCE-DRVH.DOCX</t>
-  </si>
-  <si>
-    <t>Fin: 30/06/2023</t>
-  </si>
-  <si>
-    <t>Elaboración de Acta de Cierre de Proyecto</t>
-  </si>
-  <si>
-    <t>Acta de Cierre del Proyecto</t>
-  </si>
-  <si>
-    <t>SVCE-ACP.DOCX</t>
+    <t>1 - 5 de Junio</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Helvetica Neue"/>
+        <b/>
+        <i/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">Plan de Proyecto </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Helvetica Neue"/>
+        <b/>
+        <i/>
+        <color rgb="FF000000"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>(PROJECT CHARTER)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>AAa</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">Agreagr textlist y botón para busqueda </t>
+    </r>
+  </si>
+  <si>
+    <t>Fin: 07/06/2023</t>
+  </si>
+  <si>
+    <t>Inicio: 08/05/2023</t>
   </si>
 </sst>
 </file>
@@ -570,7 +656,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="27">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -682,9 +768,33 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <i/>
       <color rgb="FF060606"/>
       <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -725,7 +835,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="37">
     <border/>
     <border>
       <left style="medium">
@@ -1071,6 +1181,58 @@
     </border>
     <border>
       <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <bottom style="medium">
@@ -1081,7 +1243,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="113">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1291,17 +1453,24 @@
     <xf borderId="19" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" textRotation="255" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="22" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="21" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" textRotation="255" vertical="center"/>
     </xf>
     <xf borderId="25" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="25" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" textRotation="255" vertical="center"/>
     </xf>
     <xf borderId="26" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
@@ -1337,7 +1506,7 @@
     <xf borderId="19" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" textRotation="255"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="25" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1347,6 +1516,49 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="31" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="32" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="34" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="28" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="35" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="36" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="28" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="32" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1362,6 +1574,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1785,12 +2001,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="50.5"/>
+    <col customWidth="1" min="2" max="2" width="17.88"/>
     <col customWidth="1" min="3" max="3" width="80.75"/>
     <col customWidth="1" min="4" max="4" width="58.75"/>
     <col customWidth="1" min="5" max="5" width="22.5"/>
@@ -2419,13 +2638,15 @@
       <c r="J34" s="72" t="s">
         <v>134</v>
       </c>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
     </row>
     <row r="35">
       <c r="A35" s="29"/>
-      <c r="B35" s="73" t="s">
+      <c r="B35" s="74" t="s">
         <v>135</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="C35" s="75" t="s">
         <v>136</v>
       </c>
       <c r="D35" s="52" t="s">
@@ -2451,7 +2672,7 @@
     <row r="36">
       <c r="A36" s="29"/>
       <c r="B36" s="45"/>
-      <c r="C36" s="74" t="s">
+      <c r="C36" s="75" t="s">
         <v>139</v>
       </c>
       <c r="D36" s="52" t="s">
@@ -2473,11 +2694,12 @@
         <v>0.0</v>
       </c>
       <c r="J36" s="45"/>
+      <c r="M36" s="76"/>
     </row>
     <row r="37" ht="18.75" customHeight="1">
       <c r="A37" s="29"/>
       <c r="B37" s="45"/>
-      <c r="C37" s="74" t="s">
+      <c r="C37" s="75" t="s">
         <v>141</v>
       </c>
       <c r="D37" s="52" t="s">
@@ -2486,7 +2708,7 @@
       <c r="E37" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="F37" s="75" t="s">
+      <c r="F37" s="77" t="s">
         <v>144</v>
       </c>
       <c r="G37" s="43">
@@ -2499,15 +2721,18 @@
         <v>0.0</v>
       </c>
       <c r="J37" s="45"/>
+      <c r="M37" s="76"/>
     </row>
     <row r="38" ht="24.0" customHeight="1">
-      <c r="A38" s="29"/>
+      <c r="A38" s="29" t="s">
+        <v>145</v>
+      </c>
       <c r="B38" s="45"/>
-      <c r="C38" s="76" t="s">
-        <v>145</v>
+      <c r="C38" s="78" t="s">
+        <v>146</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E38" s="48" t="s">
         <v>61</v>
@@ -2525,55 +2750,57 @@
         <v>0.0</v>
       </c>
       <c r="J38" s="45"/>
+      <c r="M38" s="76"/>
     </row>
     <row r="39" ht="27.75" customHeight="1">
-      <c r="A39" s="29"/>
+      <c r="A39" s="79"/>
       <c r="B39" s="45"/>
-      <c r="C39" s="77" t="s">
-        <v>147</v>
-      </c>
-      <c r="D39" s="78" t="s">
+      <c r="C39" s="80" t="s">
         <v>148</v>
       </c>
-      <c r="E39" s="79" t="s">
+      <c r="D39" s="81" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="80" t="s">
+      <c r="F39" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="G39" s="81">
+      <c r="G39" s="84">
         <v>45065.0</v>
       </c>
-      <c r="H39" s="81">
+      <c r="H39" s="84">
         <v>45080.0</v>
       </c>
-      <c r="I39" s="82">
+      <c r="I39" s="85">
         <v>0.0</v>
       </c>
       <c r="J39" s="45"/>
+      <c r="M39" s="76"/>
     </row>
     <row r="40" ht="20.25" customHeight="1">
       <c r="A40" s="29"/>
       <c r="B40" s="45"/>
-      <c r="C40" s="77" t="s">
-        <v>149</v>
-      </c>
-      <c r="D40" s="78" t="s">
+      <c r="C40" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="E40" s="79" t="s">
+      <c r="D40" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="F40" s="80" t="s">
+      <c r="F40" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="G40" s="81">
+      <c r="G40" s="84">
         <v>45065.0</v>
       </c>
-      <c r="H40" s="81">
+      <c r="H40" s="84">
         <v>45080.0</v>
       </c>
-      <c r="I40" s="82">
+      <c r="I40" s="85">
         <v>0.0</v>
       </c>
       <c r="J40" s="45"/>
@@ -2581,45 +2808,45 @@
     <row r="41" ht="23.25" customHeight="1">
       <c r="A41" s="29"/>
       <c r="B41" s="45"/>
-      <c r="C41" s="77" t="s">
-        <v>151</v>
-      </c>
-      <c r="D41" s="78" t="s">
+      <c r="C41" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="E41" s="79" t="s">
+      <c r="D41" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="F41" s="80" t="s">
+      <c r="E41" s="82" t="s">
+        <v>154</v>
+      </c>
+      <c r="F41" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="G41" s="81">
+      <c r="G41" s="84">
         <v>45066.0</v>
       </c>
-      <c r="H41" s="81">
+      <c r="H41" s="84">
         <v>45080.0</v>
       </c>
-      <c r="I41" s="82">
+      <c r="I41" s="85">
         <v>0.0</v>
       </c>
       <c r="J41" s="45"/>
     </row>
     <row r="42" ht="21.0" customHeight="1">
       <c r="A42" s="29"/>
-      <c r="B42" s="83" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" s="84" t="s">
+      <c r="B42" s="86" t="s">
         <v>155</v>
       </c>
+      <c r="C42" s="87" t="s">
+        <v>156</v>
+      </c>
       <c r="D42" s="60" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E42" s="61" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F42" s="62" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G42" s="63">
         <v>45068.0</v>
@@ -2631,22 +2858,24 @@
         <v>0.0</v>
       </c>
       <c r="J42" s="65"/>
+      <c r="L42" s="73"/>
+      <c r="M42" s="73"/>
     </row>
     <row r="43" ht="24.0" customHeight="1">
       <c r="A43" s="25"/>
       <c r="B43" s="66"/>
-      <c r="AA43" s="85"/>
+      <c r="AA43" s="88"/>
     </row>
     <row r="44" ht="22.5" customHeight="1">
       <c r="A44" s="29"/>
-      <c r="B44" s="86" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="87" t="s">
+      <c r="B44" s="89" t="s">
         <v>160</v>
       </c>
+      <c r="C44" s="90" t="s">
+        <v>161</v>
+      </c>
       <c r="D44" s="69" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E44" s="70" t="s">
         <v>61</v>
@@ -2663,20 +2892,20 @@
       <c r="I44" s="71">
         <v>0.0</v>
       </c>
-      <c r="J44" s="88" t="s">
+      <c r="J44" s="91" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="45" ht="23.25" customHeight="1">
       <c r="A45" s="29"/>
-      <c r="B45" s="73" t="s">
-        <v>162</v>
-      </c>
-      <c r="C45" s="74" t="s">
+      <c r="B45" s="74" t="s">
         <v>163</v>
       </c>
+      <c r="C45" s="75" t="s">
+        <v>164</v>
+      </c>
       <c r="D45" s="52" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E45" s="48" t="s">
         <v>61</v>
@@ -2698,11 +2927,11 @@
     <row r="46" ht="22.5" customHeight="1">
       <c r="A46" s="29"/>
       <c r="B46" s="45"/>
-      <c r="C46" s="76" t="s">
+      <c r="C46" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" s="92" t="s">
         <v>165</v>
-      </c>
-      <c r="D46" s="89" t="s">
-        <v>164</v>
       </c>
       <c r="E46" s="48" t="s">
         <v>61</v>
@@ -2724,14 +2953,14 @@
     <row r="47">
       <c r="A47" s="29"/>
       <c r="B47" s="45"/>
-      <c r="C47" s="90" t="s">
-        <v>166</v>
+      <c r="C47" s="93" t="s">
+        <v>167</v>
       </c>
       <c r="D47" s="52" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E47" s="48" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F47" s="42" t="s">
         <v>129</v>
@@ -2750,14 +2979,14 @@
     <row r="48" ht="30.75" customHeight="1">
       <c r="A48" s="29"/>
       <c r="B48" s="45"/>
-      <c r="C48" s="90" t="s">
-        <v>169</v>
+      <c r="C48" s="93" t="s">
+        <v>170</v>
       </c>
       <c r="D48" s="52" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E48" s="48" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F48" s="42" t="s">
         <v>99</v>
@@ -2765,7 +2994,7 @@
       <c r="G48" s="43">
         <v>45101.0</v>
       </c>
-      <c r="H48" s="91">
+      <c r="H48" s="94">
         <v>45105.0</v>
       </c>
       <c r="I48" s="49">
@@ -2775,17 +3004,17 @@
     </row>
     <row r="49" ht="25.5" customHeight="1">
       <c r="A49" s="29"/>
-      <c r="B49" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="92" t="s">
+      <c r="B49" s="86" t="s">
         <v>173</v>
       </c>
+      <c r="C49" s="95" t="s">
+        <v>174</v>
+      </c>
       <c r="D49" s="60" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E49" s="61" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F49" s="62" t="s">
         <v>70</v>
@@ -2801,20 +3030,1207 @@
       </c>
       <c r="J49" s="65"/>
     </row>
+    <row r="56">
+      <c r="B56" s="96" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="97" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" s="98"/>
+      <c r="C57" s="99"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="98"/>
+      <c r="C58" s="100" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" ht="18.0" customHeight="1">
+      <c r="B59" s="101"/>
+      <c r="C59" s="102"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="103"/>
+    </row>
+    <row r="61" ht="37.5" customHeight="1">
+      <c r="B61" s="96" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61" s="104" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" ht="27.75" customHeight="1">
+      <c r="B62" s="98"/>
+      <c r="C62" s="105" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" s="98"/>
+      <c r="C63" s="106" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" s="101"/>
+      <c r="C64" s="102"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="103"/>
+    </row>
+    <row r="66" ht="33.0" customHeight="1">
+      <c r="B66" s="107" t="s">
+        <v>182</v>
+      </c>
+      <c r="C66" s="104" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" ht="24.75" customHeight="1">
+      <c r="B67" s="98"/>
+      <c r="C67" s="105" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" s="98"/>
+      <c r="C68" s="106" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" s="101"/>
+      <c r="C69" s="102"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="18">
     <mergeCell ref="J14:J32"/>
     <mergeCell ref="B15:B31"/>
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="J34:J42"/>
+    <mergeCell ref="B35:B41"/>
     <mergeCell ref="B43:AA43"/>
     <mergeCell ref="J44:J49"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="C63:C64"/>
     <mergeCell ref="B45:B48"/>
-    <mergeCell ref="B35:B41"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C68:C69"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="D9"/>
   </hyperlinks>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="50.5"/>
+    <col customWidth="1" min="2" max="2" width="17.88"/>
+    <col customWidth="1" min="3" max="3" width="80.75"/>
+    <col customWidth="1" hidden="1" min="4" max="4" width="58.75"/>
+    <col customWidth="1" hidden="1" min="5" max="5" width="22.5"/>
+    <col customWidth="1" min="6" max="6" width="59.38"/>
+    <col customWidth="1" min="7" max="7" width="16.75"/>
+    <col customWidth="1" min="8" max="8" width="20.13"/>
+    <col customWidth="1" min="9" max="9" width="19.0"/>
+    <col customWidth="1" min="10" max="10" width="20.38"/>
+  </cols>
+  <sheetData>
+    <row r="3">
+      <c r="C3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="19">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="22">
+        <v>45020.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="22">
+        <v>45107.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="29"/>
+      <c r="B14" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="35">
+        <v>45020.0</v>
+      </c>
+      <c r="H14" s="35">
+        <v>45022.0</v>
+      </c>
+      <c r="I14" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="29"/>
+      <c r="B15" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="43">
+        <v>45023.0</v>
+      </c>
+      <c r="H15" s="43">
+        <v>45025.0</v>
+      </c>
+      <c r="I15" s="44">
+        <v>1.0</v>
+      </c>
+      <c r="J15" s="45"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="29"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="43">
+        <v>44661.0</v>
+      </c>
+      <c r="H16" s="43">
+        <v>45027.0</v>
+      </c>
+      <c r="I16" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J16" s="45"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="29"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H17" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="I17" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J17" s="45"/>
+    </row>
+    <row r="18" ht="20.25" customHeight="1">
+      <c r="B18" s="46"/>
+      <c r="C18" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H18" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="I18" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J18" s="45"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="29"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H19" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I19" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J19" s="45"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="29"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H20" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I20" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J20" s="45"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="29"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H21" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I21" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J21" s="45"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="29"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H22" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I22" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J22" s="45"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="29"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H23" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I23" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J23" s="45"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="29"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H24" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I24" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J24" s="45"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="29"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H25" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I25" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J25" s="45"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="29"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H26" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I26" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J26" s="45"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="29"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="43">
+        <v>45028.0</v>
+      </c>
+      <c r="H27" s="43">
+        <v>45037.0</v>
+      </c>
+      <c r="I27" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J27" s="45"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="29"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="43">
+        <v>45038.0</v>
+      </c>
+      <c r="H28" s="43">
+        <v>45038.0</v>
+      </c>
+      <c r="I28" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J28" s="45"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="29"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="43">
+        <v>45039.0</v>
+      </c>
+      <c r="H29" s="43">
+        <v>45043.0</v>
+      </c>
+      <c r="I29" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J29" s="45"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="29"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="G30" s="55">
+        <v>45044.0</v>
+      </c>
+      <c r="H30" s="43">
+        <v>45048.0</v>
+      </c>
+      <c r="I30" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J30" s="45"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="29"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="43">
+        <v>45044.0</v>
+      </c>
+      <c r="H31" s="43">
+        <v>45048.0</v>
+      </c>
+      <c r="I31" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J31" s="45"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="29"/>
+      <c r="B32" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="62" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" s="63">
+        <v>45049.0</v>
+      </c>
+      <c r="H32" s="63">
+        <v>45049.0</v>
+      </c>
+      <c r="I32" s="64">
+        <v>0.0</v>
+      </c>
+      <c r="J32" s="65"/>
+    </row>
+    <row r="33" ht="28.5" customHeight="1">
+      <c r="A33" s="29"/>
+      <c r="B33" s="66"/>
+    </row>
+    <row r="34" ht="29.25" customHeight="1">
+      <c r="A34" s="29"/>
+      <c r="B34" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" s="35">
+        <v>45050.0</v>
+      </c>
+      <c r="H34" s="35">
+        <v>45060.0</v>
+      </c>
+      <c r="I34" s="71">
+        <v>1.0</v>
+      </c>
+      <c r="J34" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="L34" s="73"/>
+      <c r="M34" s="73"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="29"/>
+      <c r="B35" s="74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="75" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="E35" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="43">
+        <v>45050.0</v>
+      </c>
+      <c r="H35" s="43">
+        <v>45060.0</v>
+      </c>
+      <c r="I35" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J35" s="45"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="29"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="43">
+        <v>45050.0</v>
+      </c>
+      <c r="H36" s="43">
+        <v>45060.0</v>
+      </c>
+      <c r="I36" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J36" s="45"/>
+      <c r="M36" s="76"/>
+    </row>
+    <row r="37" ht="18.75" customHeight="1">
+      <c r="A37" s="29"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="43">
+        <v>45061.0</v>
+      </c>
+      <c r="H37" s="43">
+        <v>45064.0</v>
+      </c>
+      <c r="I37" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J37" s="45"/>
+      <c r="M37" s="76"/>
+    </row>
+    <row r="38" ht="24.0" customHeight="1">
+      <c r="A38" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="45"/>
+      <c r="C38" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="43">
+        <v>45065.0</v>
+      </c>
+      <c r="H38" s="43">
+        <v>45080.0</v>
+      </c>
+      <c r="I38" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="J38" s="45"/>
+      <c r="M38" s="76"/>
+    </row>
+    <row r="39" ht="27.75" customHeight="1">
+      <c r="A39" s="79"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="80" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="81" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="84">
+        <v>45065.0</v>
+      </c>
+      <c r="H39" s="84">
+        <v>45080.0</v>
+      </c>
+      <c r="I39" s="85">
+        <v>1.0</v>
+      </c>
+      <c r="J39" s="45"/>
+      <c r="M39" s="76"/>
+    </row>
+    <row r="40" ht="20.25" customHeight="1">
+      <c r="A40" s="29"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="81" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="83" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" s="84">
+        <v>45065.0</v>
+      </c>
+      <c r="H40" s="84">
+        <v>45080.0</v>
+      </c>
+      <c r="I40" s="85">
+        <v>1.0</v>
+      </c>
+      <c r="J40" s="45"/>
+    </row>
+    <row r="41" ht="23.25" customHeight="1">
+      <c r="A41" s="29"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="80" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" s="81" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" s="82" t="s">
+        <v>154</v>
+      </c>
+      <c r="F41" s="83" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" s="84">
+        <v>45066.0</v>
+      </c>
+      <c r="H41" s="84">
+        <v>45080.0</v>
+      </c>
+      <c r="I41" s="85">
+        <v>1.0</v>
+      </c>
+      <c r="J41" s="45"/>
+    </row>
+    <row r="42" ht="21.0" customHeight="1">
+      <c r="A42" s="29"/>
+      <c r="B42" s="86" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" s="87" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="F42" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="63">
+        <v>45068.0</v>
+      </c>
+      <c r="H42" s="63">
+        <v>45084.0</v>
+      </c>
+      <c r="I42" s="108">
+        <v>0.0</v>
+      </c>
+      <c r="J42" s="65"/>
+      <c r="L42" s="73"/>
+      <c r="M42" s="73"/>
+    </row>
+    <row r="43" ht="24.0" customHeight="1">
+      <c r="A43" s="25"/>
+      <c r="B43" s="66"/>
+      <c r="AA43" s="88"/>
+    </row>
+    <row r="44" ht="22.5" customHeight="1">
+      <c r="A44" s="29"/>
+      <c r="B44" s="89" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" s="90" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="E44" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="G44" s="35">
+        <v>45085.0</v>
+      </c>
+      <c r="H44" s="35">
+        <v>45099.0</v>
+      </c>
+      <c r="I44" s="71">
+        <v>0.0</v>
+      </c>
+      <c r="J44" s="91" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" ht="23.25" customHeight="1">
+      <c r="A45" s="29"/>
+      <c r="B45" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" s="43">
+        <v>45085.0</v>
+      </c>
+      <c r="H45" s="43">
+        <v>45099.0</v>
+      </c>
+      <c r="I45" s="49">
+        <v>0.0</v>
+      </c>
+      <c r="J45" s="45"/>
+    </row>
+    <row r="46" ht="22.5" customHeight="1">
+      <c r="A46" s="29"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" s="92" t="s">
+        <v>165</v>
+      </c>
+      <c r="E46" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" s="43">
+        <v>45085.0</v>
+      </c>
+      <c r="H46" s="43">
+        <v>45099.0</v>
+      </c>
+      <c r="I46" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J46" s="45"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="29"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="93" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="E47" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="F47" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" s="43">
+        <v>45085.0</v>
+      </c>
+      <c r="H47" s="43">
+        <v>45100.0</v>
+      </c>
+      <c r="I47" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="J47" s="45"/>
+    </row>
+    <row r="48" ht="30.75" customHeight="1">
+      <c r="A48" s="29"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="93" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="E48" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" s="43">
+        <v>45101.0</v>
+      </c>
+      <c r="H48" s="94">
+        <v>45105.0</v>
+      </c>
+      <c r="I48" s="49">
+        <v>0.0</v>
+      </c>
+      <c r="J48" s="45"/>
+    </row>
+    <row r="49" ht="25.5" customHeight="1">
+      <c r="A49" s="29"/>
+      <c r="B49" s="86" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" s="95" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="60" t="s">
+        <v>175</v>
+      </c>
+      <c r="E49" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F49" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="G49" s="63">
+        <v>45106.0</v>
+      </c>
+      <c r="H49" s="63">
+        <v>45107.0</v>
+      </c>
+      <c r="I49" s="64">
+        <v>0.0</v>
+      </c>
+      <c r="J49" s="65"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="109"/>
+      <c r="C56" s="110"/>
+    </row>
+    <row r="58">
+      <c r="C58" s="110"/>
+    </row>
+    <row r="59" ht="18.0" customHeight="1"/>
+    <row r="60">
+      <c r="B60" s="103"/>
+    </row>
+    <row r="61" ht="37.5" customHeight="1">
+      <c r="B61" s="109"/>
+      <c r="C61" s="111"/>
+    </row>
+    <row r="62" ht="27.75" customHeight="1">
+      <c r="C62" s="111"/>
+    </row>
+    <row r="63">
+      <c r="C63" s="111"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="103"/>
+    </row>
+    <row r="66" ht="33.0" customHeight="1">
+      <c r="B66" s="112"/>
+      <c r="C66" s="111"/>
+    </row>
+    <row r="67" ht="24.75" customHeight="1">
+      <c r="C67" s="111"/>
+    </row>
+    <row r="68">
+      <c r="C68" s="111"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="J14:J32"/>
+    <mergeCell ref="B15:B31"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="J34:J42"/>
+    <mergeCell ref="B35:B41"/>
+    <mergeCell ref="B43:AA43"/>
+    <mergeCell ref="J44:J49"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D61:D62"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D9"/>
+  </hyperlinks>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
última actualización del cronograma
</commit_message>
<xml_diff>
--- a/Desarrollo/SVCE/Documentos/SVCE-CP.xlsx
+++ b/Desarrollo/SVCE/Documentos/SVCE-CP.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\NUEVAAA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDCF3A2-F651-4CC6-BFD5-8F52D3881063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="INTEGRANTES  ROLES" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name=" CRONOGRAMA" sheetId="2" r:id="rId5"/>
+    <sheet name="INTEGRANTES  ROLES" sheetId="1" r:id="rId1"/>
+    <sheet name=" CRONOGRAMA" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -220,21 +229,21 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Helvetica Neue"/>
         <b/>
         <i/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
       </rPr>
       <t xml:space="preserve">Plan de Proyecto </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Helvetica Neue"/>
         <b/>
         <i/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
       </rPr>
       <t>(PROJECT CHARTER)</t>
     </r>
@@ -468,19 +477,18 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Arial"/>
-        <b/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="12.0"/>
       </rPr>
       <t>AAa</t>
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
-        <b val="0"/>
-        <color rgb="FF000000"/>
-        <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve">Agreagr textlist y botón para busqueda </t>
     </r>
@@ -585,149 +593,178 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Georgia"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Georgia"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Georgia"/>
     </font>
-    <font/>
     <font>
-      <sz val="12.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Georgia"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Georgia"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Georgia"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
-      <sz val="22.0"/>
+      <sz val="22"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15.0"/>
+      <sz val="15"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF060606"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color rgb="FF060606"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color rgb="FF060606"/>
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -735,7 +772,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -769,7 +806,13 @@
     </fill>
   </fills>
   <borders count="35">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -783,19 +826,23 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -805,6 +852,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -819,6 +867,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -833,6 +882,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -841,9 +891,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -852,9 +904,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -863,9 +917,11 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -880,6 +936,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -894,6 +951,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -908,6 +966,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -922,6 +981,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -936,6 +996,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -950,6 +1011,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -964,6 +1026,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -978,14 +1041,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1000,6 +1067,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -1011,11 +1079,17 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -1024,14 +1098,20 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -1040,11 +1120,14 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1054,8 +1137,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1065,14 +1150,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1084,6 +1173,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1095,8 +1186,11 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1106,35 +1200,49 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1143,337 +1251,302 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="15" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="255" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="0" vertical="center"/>
-    </xf>
-    <xf borderId="15" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="98">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="255" vertical="center"/>
-    </xf>
-    <xf borderId="20" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="255" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="20" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="20" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="22" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="0" vertical="center"/>
-    </xf>
-    <xf borderId="12" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="0" vertical="center"/>
-    </xf>
-    <xf borderId="24" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" textRotation="255" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="22" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="21" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="255" vertical="center"/>
-    </xf>
-    <xf borderId="25" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="25" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" textRotation="255" vertical="center"/>
-    </xf>
-    <xf borderId="26" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="27" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="28" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="29" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="30" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="24" fillId="5" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" textRotation="255"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="25" fillId="5" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="19" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="31" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="6" fontId="19" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="32" fillId="0" fontId="14" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="33" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="34" fillId="0" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1663,25 +1736,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.25"/>
-    <col customWidth="1" min="3" max="4" width="19.88"/>
-    <col customWidth="1" min="5" max="5" width="44.88"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="2:6" ht="15.75" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1690,190 +1766,190 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="2:6">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4">
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+    <row r="4" spans="2:6">
+      <c r="B4" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="82"/>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:6">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="2:6">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:6">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:6">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:6">
+      <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="10" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="2:6">
+      <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="2:6">
+      <c r="B12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13">
-      <c r="B13" s="15" t="s">
+    <row r="13" spans="2:6">
+      <c r="B13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="13" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="2:6">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="2:6">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="2:6">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="2:6">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="2:6">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1884,1106 +1960,1161 @@
   <mergeCells count="1">
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A3:AA70"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C43" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="50.5"/>
-    <col customWidth="1" min="2" max="2" width="17.88"/>
-    <col customWidth="1" min="3" max="3" width="80.75"/>
-    <col customWidth="1" hidden="1" min="4" max="4" width="58.75"/>
-    <col customWidth="1" hidden="1" min="5" max="5" width="22.5"/>
-    <col customWidth="1" min="6" max="6" width="59.38"/>
-    <col customWidth="1" min="7" max="7" width="16.75"/>
-    <col customWidth="1" min="8" max="8" width="20.13"/>
-    <col customWidth="1" min="9" max="9" width="19.0"/>
-    <col customWidth="1" min="10" max="10" width="20.38"/>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="80.7109375" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="59.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
-      <c r="C3" s="18" t="s">
+    <row r="3" spans="1:10" ht="15">
+      <c r="C3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="19">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" s="20" t="s">
+      <c r="D3" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15">
+      <c r="C4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5">
-      <c r="C5" s="20" t="s">
+    <row r="5" spans="1:10" ht="15">
+      <c r="C5" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6">
-      <c r="C6" s="20" t="s">
+    <row r="6" spans="1:10" ht="15">
+      <c r="C6" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7">
-      <c r="C7" s="20" t="s">
+    <row r="7" spans="1:10" ht="15">
+      <c r="C7" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="22">
-        <v>45020.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" s="20" t="s">
+      <c r="D7" s="18">
+        <v>45020</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15">
+      <c r="C8" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="22">
-        <v>45107.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" s="23" t="s">
+      <c r="D8" s="18">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15">
+      <c r="C9" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30" t="s">
+    <row r="14" spans="1:10" ht="25.5">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="35">
-        <v>45020.0</v>
-      </c>
-      <c r="H14" s="35">
-        <v>45022.0</v>
-      </c>
-      <c r="I14" s="36">
-        <v>1.0</v>
-      </c>
-      <c r="J14" s="37" t="s">
+      <c r="G14" s="30">
+        <v>45020</v>
+      </c>
+      <c r="H14" s="30">
+        <v>45022</v>
+      </c>
+      <c r="I14" s="31">
+        <v>1</v>
+      </c>
+      <c r="J14" s="83" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="29"/>
-      <c r="B15" s="38" t="s">
+    <row r="15" spans="1:10" ht="12.75">
+      <c r="A15" s="24"/>
+      <c r="B15" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="43">
-        <v>45023.0</v>
-      </c>
-      <c r="H15" s="43">
-        <v>45025.0</v>
-      </c>
-      <c r="I15" s="44">
-        <v>1.0</v>
-      </c>
-      <c r="J15" s="45"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="29"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="39" t="s">
+      <c r="G15" s="36">
+        <v>45023</v>
+      </c>
+      <c r="H15" s="36">
+        <v>45025</v>
+      </c>
+      <c r="I15" s="37">
+        <v>1</v>
+      </c>
+      <c r="J15" s="84"/>
+    </row>
+    <row r="16" spans="1:10" ht="12.75">
+      <c r="A16" s="24"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="43">
-        <v>44661.0</v>
-      </c>
-      <c r="H16" s="43">
-        <v>45027.0</v>
-      </c>
-      <c r="I16" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J16" s="45"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="29"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="39" t="s">
+      <c r="G16" s="36">
+        <v>44661</v>
+      </c>
+      <c r="H16" s="36">
+        <v>45027</v>
+      </c>
+      <c r="I16" s="37">
+        <v>1</v>
+      </c>
+      <c r="J16" s="84"/>
+    </row>
+    <row r="17" spans="1:10" ht="12.75">
+      <c r="A17" s="24"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H17" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="I17" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J17" s="45"/>
-    </row>
-    <row r="18" ht="20.25" customHeight="1">
-      <c r="B18" s="46"/>
-      <c r="C18" s="39" t="s">
+      <c r="G17" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H17" s="36">
+        <v>45028</v>
+      </c>
+      <c r="I17" s="37">
+        <v>1</v>
+      </c>
+      <c r="J17" s="84"/>
+    </row>
+    <row r="18" spans="1:10" ht="20.25" customHeight="1">
+      <c r="B18" s="87"/>
+      <c r="C18" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H18" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="I18" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J18" s="45"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="29"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="51" t="s">
+      <c r="G18" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H18" s="36">
+        <v>45028</v>
+      </c>
+      <c r="I18" s="37">
+        <v>1</v>
+      </c>
+      <c r="J18" s="84"/>
+    </row>
+    <row r="19" spans="1:10" ht="12.75">
+      <c r="A19" s="24"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H19" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I19" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J19" s="45"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="29"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="51" t="s">
+      <c r="G19" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H19" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I19" s="37">
+        <v>1</v>
+      </c>
+      <c r="J19" s="84"/>
+    </row>
+    <row r="20" spans="1:10" ht="12.75">
+      <c r="A20" s="24"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="52" t="s">
+      <c r="D20" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H20" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I20" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J20" s="45"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="29"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="51" t="s">
+      <c r="G20" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H20" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I20" s="37">
+        <v>1</v>
+      </c>
+      <c r="J20" s="84"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75">
+      <c r="A21" s="24"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="52" t="s">
+      <c r="D21" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H21" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I21" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J21" s="45"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="29"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="51" t="s">
+      <c r="G21" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H21" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I21" s="37">
+        <v>1</v>
+      </c>
+      <c r="J21" s="84"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.75">
+      <c r="A22" s="24"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H22" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I22" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J22" s="45"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="29"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="51" t="s">
+      <c r="G22" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H22" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I22" s="37">
+        <v>1</v>
+      </c>
+      <c r="J22" s="84"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.75">
+      <c r="A23" s="24"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="52" t="s">
+      <c r="D23" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H23" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I23" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J23" s="45"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="29"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="51" t="s">
+      <c r="G23" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H23" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I23" s="37">
+        <v>1</v>
+      </c>
+      <c r="J23" s="84"/>
+    </row>
+    <row r="24" spans="1:10" ht="12.75">
+      <c r="A24" s="24"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="52" t="s">
+      <c r="D24" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="42" t="s">
+      <c r="F24" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H24" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I24" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J24" s="45"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="51" t="s">
+      <c r="G24" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H24" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I24" s="37">
+        <v>1</v>
+      </c>
+      <c r="J24" s="84"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.75">
+      <c r="A25" s="24"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="52" t="s">
+      <c r="D25" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="42" t="s">
+      <c r="F25" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H25" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I25" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J25" s="45"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="29"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="51" t="s">
+      <c r="G25" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H25" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I25" s="37">
+        <v>1</v>
+      </c>
+      <c r="J25" s="84"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.75">
+      <c r="A26" s="24"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H26" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I26" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J26" s="45"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="29"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="51" t="s">
+      <c r="G26" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H26" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I26" s="37">
+        <v>1</v>
+      </c>
+      <c r="J26" s="84"/>
+    </row>
+    <row r="27" spans="1:10" ht="12.75">
+      <c r="A27" s="24"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="43">
-        <v>45028.0</v>
-      </c>
-      <c r="H27" s="43">
-        <v>45037.0</v>
-      </c>
-      <c r="I27" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J27" s="45"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="29"/>
-      <c r="B28" s="46"/>
-      <c r="C28" s="51" t="s">
+      <c r="G27" s="36">
+        <v>45028</v>
+      </c>
+      <c r="H27" s="36">
+        <v>45037</v>
+      </c>
+      <c r="I27" s="37">
+        <v>1</v>
+      </c>
+      <c r="J27" s="84"/>
+    </row>
+    <row r="28" spans="1:10" ht="25.5">
+      <c r="A28" s="24"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="52" t="s">
+      <c r="D28" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="F28" s="42" t="s">
+      <c r="F28" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="43">
-        <v>45038.0</v>
-      </c>
-      <c r="H28" s="43">
-        <v>45038.0</v>
-      </c>
-      <c r="I28" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J28" s="45"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="29"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="53" t="s">
+      <c r="G28" s="36">
+        <v>45038</v>
+      </c>
+      <c r="H28" s="36">
+        <v>45038</v>
+      </c>
+      <c r="I28" s="37">
+        <v>1</v>
+      </c>
+      <c r="J28" s="84"/>
+    </row>
+    <row r="29" spans="1:10" ht="12.75">
+      <c r="A29" s="24"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="52" t="s">
+      <c r="D29" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="F29" s="42" t="s">
+      <c r="F29" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="G29" s="43">
-        <v>45039.0</v>
-      </c>
-      <c r="H29" s="43">
-        <v>45043.0</v>
-      </c>
-      <c r="I29" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J29" s="45"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="29"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="54" t="s">
+      <c r="G29" s="36">
+        <v>45039</v>
+      </c>
+      <c r="H29" s="36">
+        <v>45043</v>
+      </c>
+      <c r="I29" s="37">
+        <v>1</v>
+      </c>
+      <c r="J29" s="84"/>
+    </row>
+    <row r="30" spans="1:10" ht="12.75">
+      <c r="A30" s="24"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="48" t="s">
+      <c r="E30" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="F30" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="G30" s="55">
-        <v>45044.0</v>
-      </c>
-      <c r="H30" s="43">
-        <v>45048.0</v>
-      </c>
-      <c r="I30" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J30" s="45"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="29"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="56" t="s">
+      <c r="G30" s="42">
+        <v>45044</v>
+      </c>
+      <c r="H30" s="36">
+        <v>45048</v>
+      </c>
+      <c r="I30" s="37">
+        <v>1</v>
+      </c>
+      <c r="J30" s="84"/>
+    </row>
+    <row r="31" spans="1:10" ht="12.75">
+      <c r="A31" s="24"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="57" t="s">
+      <c r="D31" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="48" t="s">
+      <c r="E31" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="F31" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="43">
-        <v>45044.0</v>
-      </c>
-      <c r="H31" s="43">
-        <v>45048.0</v>
-      </c>
-      <c r="I31" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J31" s="45"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="29"/>
-      <c r="B32" s="58" t="s">
+      <c r="G31" s="36">
+        <v>45044</v>
+      </c>
+      <c r="H31" s="36">
+        <v>45048</v>
+      </c>
+      <c r="I31" s="37">
+        <v>1</v>
+      </c>
+      <c r="J31" s="84"/>
+    </row>
+    <row r="32" spans="1:10" ht="25.5">
+      <c r="A32" s="24"/>
+      <c r="B32" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="59" t="s">
+      <c r="C32" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="61" t="s">
+      <c r="E32" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="F32" s="62" t="s">
+      <c r="F32" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="G32" s="63">
-        <v>45049.0</v>
-      </c>
-      <c r="H32" s="63">
-        <v>45049.0</v>
-      </c>
-      <c r="I32" s="64">
-        <v>0.0</v>
-      </c>
-      <c r="J32" s="65"/>
-    </row>
-    <row r="33" ht="28.5" customHeight="1">
-      <c r="A33" s="29"/>
-      <c r="B33" s="66"/>
-    </row>
-    <row r="34" ht="29.25" customHeight="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="67" t="s">
+      <c r="G32" s="50">
+        <v>45049</v>
+      </c>
+      <c r="H32" s="50">
+        <v>45049</v>
+      </c>
+      <c r="I32" s="51">
+        <v>0</v>
+      </c>
+      <c r="J32" s="85"/>
+    </row>
+    <row r="33" spans="1:27" ht="28.5" customHeight="1">
+      <c r="A33" s="24"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="89"/>
+    </row>
+    <row r="34" spans="1:27" ht="29.25" customHeight="1">
+      <c r="A34" s="24"/>
+      <c r="B34" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="C34" s="68" t="s">
+      <c r="C34" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="D34" s="69" t="s">
+      <c r="D34" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="E34" s="70" t="s">
+      <c r="E34" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="G34" s="35">
-        <v>45050.0</v>
-      </c>
-      <c r="H34" s="35">
-        <v>45060.0</v>
-      </c>
-      <c r="I34" s="71">
-        <v>1.0</v>
-      </c>
-      <c r="J34" s="72" t="s">
+      <c r="G34" s="30">
+        <v>45050</v>
+      </c>
+      <c r="H34" s="30">
+        <v>45060</v>
+      </c>
+      <c r="I34" s="31">
+        <v>1</v>
+      </c>
+      <c r="J34" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="29"/>
-      <c r="B35" s="74" t="s">
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+    </row>
+    <row r="35" spans="1:27" ht="12.75">
+      <c r="A35" s="24"/>
+      <c r="B35" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="E35" s="48" t="s">
+      <c r="E35" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="42" t="s">
+      <c r="F35" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="G35" s="43">
-        <v>45050.0</v>
-      </c>
-      <c r="H35" s="43">
-        <v>45060.0</v>
-      </c>
-      <c r="I35" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J35" s="45"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="29"/>
-      <c r="B36" s="45"/>
-      <c r="C36" s="75" t="s">
+      <c r="G35" s="36">
+        <v>45050</v>
+      </c>
+      <c r="H35" s="36">
+        <v>45060</v>
+      </c>
+      <c r="I35" s="37">
+        <v>1</v>
+      </c>
+      <c r="J35" s="84"/>
+    </row>
+    <row r="36" spans="1:27" ht="12.75">
+      <c r="A36" s="24"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="E36" s="48" t="s">
+      <c r="E36" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="42" t="s">
+      <c r="F36" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="G36" s="43">
-        <v>45050.0</v>
-      </c>
-      <c r="H36" s="43">
-        <v>45060.0</v>
-      </c>
-      <c r="I36" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J36" s="45"/>
-      <c r="M36" s="76"/>
-    </row>
-    <row r="37" ht="18.75" customHeight="1">
-      <c r="A37" s="29"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="75" t="s">
+      <c r="G36" s="36">
+        <v>45050</v>
+      </c>
+      <c r="H36" s="36">
+        <v>45060</v>
+      </c>
+      <c r="I36" s="37">
+        <v>1</v>
+      </c>
+      <c r="J36" s="84"/>
+      <c r="M36" s="58"/>
+    </row>
+    <row r="37" spans="1:27" ht="18.75" customHeight="1">
+      <c r="A37" s="24"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="D37" s="52" t="s">
+      <c r="D37" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="48" t="s">
+      <c r="E37" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="77" t="s">
+      <c r="F37" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="G37" s="43">
-        <v>45061.0</v>
-      </c>
-      <c r="H37" s="43">
-        <v>45064.0</v>
-      </c>
-      <c r="I37" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J37" s="45"/>
-      <c r="M37" s="76"/>
-    </row>
-    <row r="38" ht="24.0" customHeight="1">
-      <c r="A38" s="29" t="s">
+      <c r="G37" s="36">
+        <v>45061</v>
+      </c>
+      <c r="H37" s="36">
+        <v>45064</v>
+      </c>
+      <c r="I37" s="37">
+        <v>1</v>
+      </c>
+      <c r="J37" s="84"/>
+      <c r="M37" s="58"/>
+    </row>
+    <row r="38" spans="1:27" ht="24" customHeight="1">
+      <c r="A38" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="78" t="s">
+      <c r="B38" s="84"/>
+      <c r="C38" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="52" t="s">
+      <c r="D38" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="48" t="s">
+      <c r="E38" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F38" s="42" t="s">
+      <c r="F38" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="G38" s="43">
-        <v>45065.0</v>
-      </c>
-      <c r="H38" s="43">
-        <v>45080.0</v>
-      </c>
-      <c r="I38" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J38" s="45"/>
-      <c r="M38" s="76"/>
-    </row>
-    <row r="39" ht="27.75" customHeight="1">
-      <c r="A39" s="79"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="80" t="s">
+      <c r="G38" s="36">
+        <v>45065</v>
+      </c>
+      <c r="H38" s="36">
+        <v>45080</v>
+      </c>
+      <c r="I38" s="37">
+        <v>1</v>
+      </c>
+      <c r="J38" s="84"/>
+      <c r="M38" s="58"/>
+    </row>
+    <row r="39" spans="1:27" ht="27.75" customHeight="1">
+      <c r="A39" s="61"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="81" t="s">
+      <c r="D39" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="E39" s="82" t="s">
+      <c r="E39" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="83" t="s">
+      <c r="F39" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="G39" s="84">
-        <v>45065.0</v>
-      </c>
-      <c r="H39" s="84">
-        <v>45080.0</v>
-      </c>
-      <c r="I39" s="85">
-        <v>1.0</v>
-      </c>
-      <c r="J39" s="45"/>
-      <c r="M39" s="76"/>
-    </row>
-    <row r="40" ht="20.25" customHeight="1">
-      <c r="A40" s="29"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="80" t="s">
+      <c r="G39" s="66">
+        <v>45065</v>
+      </c>
+      <c r="H39" s="66">
+        <v>45080</v>
+      </c>
+      <c r="I39" s="67">
+        <v>1</v>
+      </c>
+      <c r="J39" s="84"/>
+      <c r="M39" s="58"/>
+    </row>
+    <row r="40" spans="1:27" ht="20.25" customHeight="1">
+      <c r="A40" s="24"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="D40" s="81" t="s">
+      <c r="D40" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="E40" s="82" t="s">
+      <c r="E40" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="F40" s="83" t="s">
+      <c r="F40" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="G40" s="84">
-        <v>45065.0</v>
-      </c>
-      <c r="H40" s="84">
-        <v>45080.0</v>
-      </c>
-      <c r="I40" s="85">
-        <v>1.0</v>
-      </c>
-      <c r="J40" s="45"/>
-    </row>
-    <row r="41" ht="23.25" customHeight="1">
-      <c r="A41" s="29"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="80" t="s">
+      <c r="G40" s="66">
+        <v>45065</v>
+      </c>
+      <c r="H40" s="66">
+        <v>45080</v>
+      </c>
+      <c r="I40" s="67">
+        <v>1</v>
+      </c>
+      <c r="J40" s="84"/>
+    </row>
+    <row r="41" spans="1:27" ht="23.25" customHeight="1">
+      <c r="A41" s="24"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="D41" s="81" t="s">
+      <c r="D41" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="E41" s="82" t="s">
+      <c r="E41" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="F41" s="83" t="s">
+      <c r="F41" s="65" t="s">
         <v>143</v>
       </c>
-      <c r="G41" s="84">
-        <v>45066.0</v>
-      </c>
-      <c r="H41" s="84">
-        <v>45080.0</v>
-      </c>
-      <c r="I41" s="85">
-        <v>1.0</v>
-      </c>
-      <c r="J41" s="45"/>
-    </row>
-    <row r="42" ht="21.0" customHeight="1">
-      <c r="A42" s="29"/>
-      <c r="B42" s="86" t="s">
+      <c r="G41" s="66">
+        <v>45066</v>
+      </c>
+      <c r="H41" s="66">
+        <v>45080</v>
+      </c>
+      <c r="I41" s="67">
+        <v>1</v>
+      </c>
+      <c r="J41" s="84"/>
+    </row>
+    <row r="42" spans="1:27" ht="21" customHeight="1">
+      <c r="A42" s="24"/>
+      <c r="B42" s="68" t="s">
         <v>154</v>
       </c>
-      <c r="C42" s="87" t="s">
+      <c r="C42" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="D42" s="60" t="s">
+      <c r="D42" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="E42" s="61" t="s">
+      <c r="E42" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="F42" s="62" t="s">
+      <c r="F42" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="G42" s="63">
-        <v>45068.0</v>
-      </c>
-      <c r="H42" s="63">
-        <v>45084.0</v>
-      </c>
-      <c r="I42" s="88">
-        <v>1.0</v>
-      </c>
-      <c r="J42" s="65"/>
-      <c r="L42" s="73"/>
-      <c r="M42" s="73"/>
-    </row>
-    <row r="43" ht="24.0" customHeight="1">
-      <c r="A43" s="25"/>
-      <c r="B43" s="66"/>
-      <c r="AA43" s="89"/>
-    </row>
-    <row r="44" ht="30.0" customHeight="1">
-      <c r="A44" s="29"/>
-      <c r="B44" s="90" t="s">
+      <c r="G42" s="50">
+        <v>45068</v>
+      </c>
+      <c r="H42" s="50">
+        <v>45084</v>
+      </c>
+      <c r="I42" s="51">
+        <v>1</v>
+      </c>
+      <c r="J42" s="85"/>
+      <c r="L42" s="55"/>
+      <c r="M42" s="55"/>
+    </row>
+    <row r="43" spans="1:27" ht="24" customHeight="1">
+      <c r="A43" s="21"/>
+      <c r="B43" s="88"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="89"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
+      <c r="I43" s="89"/>
+      <c r="J43" s="89"/>
+      <c r="K43" s="89"/>
+      <c r="L43" s="89"/>
+      <c r="M43" s="89"/>
+      <c r="N43" s="89"/>
+      <c r="O43" s="89"/>
+      <c r="P43" s="89"/>
+      <c r="Q43" s="89"/>
+      <c r="R43" s="89"/>
+      <c r="S43" s="89"/>
+      <c r="T43" s="89"/>
+      <c r="U43" s="89"/>
+      <c r="V43" s="89"/>
+      <c r="W43" s="89"/>
+      <c r="X43" s="89"/>
+      <c r="Y43" s="89"/>
+      <c r="Z43" s="89"/>
+      <c r="AA43" s="92"/>
+    </row>
+    <row r="44" spans="1:27" ht="30" customHeight="1">
+      <c r="A44" s="24"/>
+      <c r="B44" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="C44" s="91" t="s">
+      <c r="C44" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="D44" s="69" t="s">
+      <c r="D44" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="E44" s="70" t="s">
+      <c r="E44" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F44" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="G44" s="35">
-        <v>45085.0</v>
-      </c>
-      <c r="H44" s="35">
-        <v>45099.0</v>
-      </c>
-      <c r="I44" s="71">
-        <v>1.0</v>
-      </c>
-      <c r="J44" s="92" t="s">
+      <c r="G44" s="30">
+        <v>45085</v>
+      </c>
+      <c r="H44" s="30">
+        <v>45099</v>
+      </c>
+      <c r="I44" s="31">
+        <v>1</v>
+      </c>
+      <c r="J44" s="93" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="45" ht="23.25" customHeight="1">
-      <c r="A45" s="29"/>
-      <c r="B45" s="74" t="s">
+    <row r="45" spans="1:27" ht="23.25" customHeight="1">
+      <c r="A45" s="24"/>
+      <c r="B45" s="91" t="s">
         <v>162</v>
       </c>
-      <c r="C45" s="75" t="s">
+      <c r="C45" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="D45" s="52" t="s">
+      <c r="D45" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="E45" s="48" t="s">
+      <c r="E45" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F45" s="42" t="s">
+      <c r="F45" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="G45" s="43">
-        <v>45085.0</v>
-      </c>
-      <c r="H45" s="43">
-        <v>45099.0</v>
-      </c>
-      <c r="I45" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J45" s="45"/>
-    </row>
-    <row r="46" ht="22.5" customHeight="1">
-      <c r="A46" s="29"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="78" t="s">
+      <c r="G45" s="36">
+        <v>45085</v>
+      </c>
+      <c r="H45" s="36">
+        <v>45099</v>
+      </c>
+      <c r="I45" s="37">
+        <v>1</v>
+      </c>
+      <c r="J45" s="84"/>
+    </row>
+    <row r="46" spans="1:27" ht="22.5" customHeight="1">
+      <c r="A46" s="24"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="D46" s="93" t="s">
+      <c r="D46" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="E46" s="48" t="s">
+      <c r="E46" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F46" s="42" t="s">
+      <c r="F46" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G46" s="43">
-        <v>45085.0</v>
-      </c>
-      <c r="H46" s="43">
-        <v>45099.0</v>
-      </c>
-      <c r="I46" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J46" s="45"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="29"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="94" t="s">
+      <c r="G46" s="36">
+        <v>45085</v>
+      </c>
+      <c r="H46" s="36">
+        <v>45099</v>
+      </c>
+      <c r="I46" s="37">
+        <v>1</v>
+      </c>
+      <c r="J46" s="84"/>
+    </row>
+    <row r="47" spans="1:27" ht="25.5">
+      <c r="A47" s="24"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="D47" s="52" t="s">
+      <c r="D47" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E47" s="48" t="s">
+      <c r="E47" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="F47" s="42" t="s">
+      <c r="F47" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="G47" s="43">
-        <v>45085.0</v>
-      </c>
-      <c r="H47" s="43">
-        <v>45100.0</v>
-      </c>
-      <c r="I47" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J47" s="45"/>
-    </row>
-    <row r="48" ht="30.75" customHeight="1">
-      <c r="A48" s="29"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="94" t="s">
+      <c r="G47" s="36">
+        <v>45085</v>
+      </c>
+      <c r="H47" s="36">
+        <v>45100</v>
+      </c>
+      <c r="I47" s="37">
+        <v>1</v>
+      </c>
+      <c r="J47" s="84"/>
+    </row>
+    <row r="48" spans="1:27" ht="30.75" customHeight="1">
+      <c r="A48" s="24"/>
+      <c r="B48" s="84"/>
+      <c r="C48" s="72" t="s">
         <v>169</v>
       </c>
-      <c r="D48" s="52" t="s">
+      <c r="D48" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="E48" s="48" t="s">
+      <c r="E48" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="F48" s="42" t="s">
+      <c r="F48" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G48" s="43">
-        <v>45101.0</v>
-      </c>
-      <c r="H48" s="95">
-        <v>45105.0</v>
-      </c>
-      <c r="I48" s="49">
-        <v>1.0</v>
-      </c>
-      <c r="J48" s="45"/>
-    </row>
-    <row r="49" ht="30.75" customHeight="1">
-      <c r="A49" s="29"/>
-      <c r="B49" s="74"/>
-      <c r="C49" s="94" t="s">
+      <c r="G48" s="36">
+        <v>45101</v>
+      </c>
+      <c r="H48" s="73">
+        <v>45105</v>
+      </c>
+      <c r="I48" s="37">
+        <v>1</v>
+      </c>
+      <c r="J48" s="84"/>
+    </row>
+    <row r="49" spans="1:10" ht="30.75" customHeight="1">
+      <c r="A49" s="24"/>
+      <c r="B49" s="56"/>
+      <c r="C49" s="72" t="s">
         <v>172</v>
       </c>
-      <c r="D49" s="81"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="83" t="s">
+      <c r="D49" s="63"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="G49" s="96">
-        <v>45106.0</v>
-      </c>
-      <c r="H49" s="97">
-        <v>45110.0</v>
-      </c>
-      <c r="I49" s="98">
-        <v>0.0</v>
-      </c>
-      <c r="J49" s="45"/>
-    </row>
-    <row r="50" ht="25.5" customHeight="1">
-      <c r="A50" s="29"/>
-      <c r="B50" s="86" t="s">
+      <c r="G49" s="74">
+        <v>45106</v>
+      </c>
+      <c r="H49" s="75">
+        <v>45110</v>
+      </c>
+      <c r="I49" s="76">
+        <v>1</v>
+      </c>
+      <c r="J49" s="84"/>
+    </row>
+    <row r="50" spans="1:10" ht="25.5" customHeight="1">
+      <c r="A50" s="24"/>
+      <c r="B50" s="68" t="s">
         <v>173</v>
       </c>
-      <c r="C50" s="99" t="s">
+      <c r="C50" s="77" t="s">
         <v>174</v>
       </c>
-      <c r="D50" s="60" t="s">
+      <c r="D50" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="E50" s="61" t="s">
+      <c r="E50" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="F50" s="62" t="s">
+      <c r="F50" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="G50" s="63">
-        <v>45106.0</v>
-      </c>
-      <c r="H50" s="100">
-        <v>45110.0</v>
-      </c>
-      <c r="I50" s="64">
-        <v>0.0</v>
-      </c>
-      <c r="J50" s="65"/>
-    </row>
-    <row r="57">
-      <c r="B57" s="101"/>
-      <c r="C57" s="102"/>
-    </row>
-    <row r="59">
-      <c r="C59" s="102"/>
-    </row>
-    <row r="60" ht="18.0" customHeight="1"/>
-    <row r="61">
-      <c r="B61" s="103"/>
-    </row>
-    <row r="62" ht="37.5" customHeight="1">
-      <c r="B62" s="101"/>
-      <c r="C62" s="104"/>
-    </row>
-    <row r="63" ht="27.75" customHeight="1">
-      <c r="C63" s="104"/>
-    </row>
-    <row r="64">
-      <c r="C64" s="104"/>
-    </row>
-    <row r="66">
-      <c r="B66" s="103"/>
-    </row>
-    <row r="67" ht="33.0" customHeight="1">
-      <c r="B67" s="105"/>
-      <c r="C67" s="104"/>
-    </row>
-    <row r="68" ht="24.75" customHeight="1">
-      <c r="C68" s="104"/>
-    </row>
-    <row r="69">
-      <c r="C69" s="104"/>
+      <c r="G50" s="50">
+        <v>45106</v>
+      </c>
+      <c r="H50" s="78">
+        <v>45110</v>
+      </c>
+      <c r="I50" s="51">
+        <v>1</v>
+      </c>
+      <c r="J50" s="85"/>
+    </row>
+    <row r="57" spans="1:10" ht="12.75">
+      <c r="B57" s="94"/>
+      <c r="C57" s="97"/>
+      <c r="D57" s="89"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B58" s="89"/>
+      <c r="C58" s="89"/>
+      <c r="D58" s="89"/>
+    </row>
+    <row r="59" spans="1:10" ht="12.75">
+      <c r="B59" s="89"/>
+      <c r="C59" s="97"/>
+      <c r="D59" s="89"/>
+    </row>
+    <row r="60" spans="1:10" ht="18" customHeight="1">
+      <c r="B60" s="89"/>
+      <c r="C60" s="89"/>
+      <c r="D60" s="89"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="B61" s="79"/>
+    </row>
+    <row r="62" spans="1:10" ht="37.5" customHeight="1">
+      <c r="B62" s="94"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="89"/>
+    </row>
+    <row r="63" spans="1:10" ht="27.75" customHeight="1">
+      <c r="B63" s="89"/>
+      <c r="C63" s="80"/>
+      <c r="D63" s="89"/>
+    </row>
+    <row r="64" spans="1:10" ht="12.75">
+      <c r="B64" s="89"/>
+      <c r="C64" s="95"/>
+    </row>
+    <row r="65" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B65" s="89"/>
+      <c r="C65" s="89"/>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" s="79"/>
+    </row>
+    <row r="67" spans="2:3" ht="33" customHeight="1">
+      <c r="B67" s="96"/>
+      <c r="C67" s="80"/>
+    </row>
+    <row r="68" spans="2:3" ht="24.75" customHeight="1">
+      <c r="B68" s="89"/>
+      <c r="C68" s="80"/>
+    </row>
+    <row r="69" spans="2:3" ht="12.75">
+      <c r="B69" s="89"/>
+      <c r="C69" s="95"/>
+    </row>
+    <row r="70" spans="2:3" ht="15.75" customHeight="1">
+      <c r="B70" s="89"/>
+      <c r="C70" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J14:J32"/>
-    <mergeCell ref="B15:B31"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="J34:J42"/>
-    <mergeCell ref="B35:B41"/>
     <mergeCell ref="B43:AA43"/>
     <mergeCell ref="J44:J50"/>
     <mergeCell ref="B62:B65"/>
@@ -2997,13 +3128,17 @@
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="D59:D60"/>
     <mergeCell ref="D62:D63"/>
+    <mergeCell ref="J14:J32"/>
+    <mergeCell ref="B15:B31"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="J34:J42"/>
+    <mergeCell ref="B35:B41"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D9"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId2"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>